<commit_message>
v1.3 add missing samples
</commit_message>
<xml_diff>
--- a/modified.xlsx
+++ b/modified.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,11 @@
           <t>Market Value</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Assets - Total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -466,6 +471,9 @@
       <c r="D2" t="n">
         <v>1108.0756</v>
       </c>
+      <c r="E2" t="n">
+        <v>2199.5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -482,6 +490,9 @@
       <c r="D3" t="n">
         <v>984.0509400000001</v>
       </c>
+      <c r="E3" t="n">
+        <v>1515</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -498,6 +509,9 @@
       <c r="D4" t="n">
         <v>907.39935</v>
       </c>
+      <c r="E4" t="n">
+        <v>1442.1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -513,6 +527,9 @@
       </c>
       <c r="D5" t="n">
         <v>1363.99164</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1524.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>